<commit_message>
Se modifico el archivo Cauca_Bateria de indicadores
</commit_message>
<xml_diff>
--- a/data/Cauca_Bateria de indicadores V1 .xlsx
+++ b/data/Cauca_Bateria de indicadores V1 .xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fupedu-my.sharepoint.com/personal/andres_pena_estudiante_fup_edu_co/Documents/Andres ING. SISTEMAS/8vo semestre/Practica empresarial/Bateria de indicadores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="8_{D47914B7-FC41-4C4A-A304-FCF069ADFF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA283D03-0DF6-4A58-B25A-B4FD85CDC507}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="8_{D47914B7-FC41-4C4A-A304-FCF069ADFF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC48C9A5-5DD8-4BF7-BA82-F1C13763C0FC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Salud y derechos sexuales y rep" sheetId="5" r:id="rId1"/>
-    <sheet name="Vida libre de violencias" sheetId="2" r:id="rId2"/>
-    <sheet name="Educacion" sheetId="4" r:id="rId3"/>
-    <sheet name="Participación social y politica" sheetId="3" r:id="rId4"/>
-    <sheet name="Autonomia ecomica" sheetId="1" r:id="rId5"/>
-    <sheet name="Paz y seguridad" sheetId="6" r:id="rId6"/>
-    <sheet name="Mujer tierra y territorio" sheetId="7" r:id="rId7"/>
-    <sheet name="Sociodemografico" sheetId="8" r:id="rId8"/>
+    <sheet name="Sociodemografico" sheetId="8" r:id="rId1"/>
+    <sheet name="Salud y derechos sexuales y rep" sheetId="5" r:id="rId2"/>
+    <sheet name="Vida libre de violencias" sheetId="2" r:id="rId3"/>
+    <sheet name="Educacion" sheetId="4" r:id="rId4"/>
+    <sheet name="Participación social y politica" sheetId="3" r:id="rId5"/>
+    <sheet name="Autonomia ecomica" sheetId="1" r:id="rId6"/>
+    <sheet name="Paz y seguridad" sheetId="6" r:id="rId7"/>
+    <sheet name="Mujer tierra y territorio" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="564">
   <si>
     <t>Bateria de indicadores OBSERVATORIO DE ASUNTOS DE LAS MUJERES DEL DEPARTAMENTO DEL CAUCA</t>
   </si>
@@ -737,10 +737,6 @@
 InfoCancer</t>
   </si>
   <si>
-    <t>https://www.sispro.gov.co/observatorios/oncancer/Paginas/Observatorio-Nacional-de-Cancer.aspx
-https://www.infocancer.co/portal/#!/filtro_mortalidad/</t>
-  </si>
-  <si>
     <t>El Ministerio de Salud y Protección Social publica la información anual sobre esta tasa en el sitio web del Observatorio Nacional de Cáncer. La publicación de los datos oficiales anuales de mortalidad por cáncer presenta un rezago de un año.</t>
   </si>
   <si>
@@ -1520,18 +1516,9 @@
     <t>SD03</t>
   </si>
   <si>
-    <t>Envejecimiento de la población</t>
-  </si>
-  <si>
-    <t>Indicador de Envejecimiento Poblacional</t>
-  </si>
-  <si>
     <t>Medir el grado de envejecimiento de la población a partir de la proporción de personas consideradas adultas mayores en relación con el total de habitantes, diferenciando por sexo</t>
   </si>
   <si>
-    <t>https://www.arcgis.com/apps/dashboards/105ba51b48f148f7b4ff21f21ea31b32</t>
-  </si>
-  <si>
     <t>SD04</t>
   </si>
   <si>
@@ -1647,9 +1634,6 @@
   </si>
   <si>
     <t xml:space="preserve">Porcentaje de mortalidad por grupo etnico en el departamento del cauca. </t>
-  </si>
-  <si>
-    <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/salud/nacimientos-y-defunciones   https://microdatos.dane.gov.co/index.php/catalog/876/data-dictionary/F35?file_name=nac2023</t>
   </si>
   <si>
     <t>Tasa de exámenes medicolegales por presunto delito sexual, según el sexo, grupo etarios, características específicas, presunto agresor, escenarios del hecho, pertenencia étnica en el dpto. del Cauca.</t>
@@ -1905,13 +1889,7 @@
     <t>Encuesta Nacional de Calidad de Vida para población campesina 2024</t>
   </si>
   <si>
-    <t>https://www.medicinalegal.gov.co/cifras-estadisticas/forensis https://www.medicinalegal.gov.co/indicadores-procuraduria</t>
-  </si>
-  <si>
     <t>Tasa de Homicidios (Basada en reporte de homicidios de la Policía Nacional)</t>
-  </si>
-  <si>
-    <t>http://microdatos.dane.gov.co/index.php/catalog/701/get_microdata https://microdatos.dane.gov.co/index.php/catalog/853/data-dictionary/F1?file_name=Caracteristicas%20generales,%20seguridad%20social%20en%20salud%20y%20educacion</t>
   </si>
   <si>
     <t>https://estadisticaselectorales.registraduria.gov.co/unit?str_opc=Elecciones%20Territoriales%20Alcald%C3%ADa&amp;idFilter=3&amp;filter=TERRITORIALES&amp;t=TERRITORIALES&amp;y1=2023&amp;i1=41&amp;y2=false&amp;i2=0</t>
@@ -2008,10 +1986,6 @@
     <t>Tablero Power BI</t>
   </si>
   <si>
-    <t>https://www.datos.gov.co/Salud-y-Protecci-n-Social/Indicadores-mortalidad-y-morbilidad-seg-n-departam/4e4i-ua65/about_data
-https://geoportal.dane.gov.co/geovisores/sociedad/estadisticas-vitales/</t>
-  </si>
-  <si>
     <t>CSV, XLS, XML</t>
   </si>
   <si>
@@ -2111,12 +2085,148 @@
   <si>
     <t>Tablero de control de demografía con los indicadores vejez y envejecimiento y Proyecciones de población - DANE</t>
   </si>
+  <si>
+    <t>Ministerio de Salud y Protección Social – SISPRO                DANE – Proyecciones de población</t>
+  </si>
+  <si>
+    <t>Tablero, XLS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.arcgis.com/apps/dashboards/105ba51b48f148f7b4ff21f21ea31b32 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/demografia-y-poblacion/proyecciones-de-poblacion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.sispro.gov.co/observatorios/oncancer/Paginas/Observatorio-Nacional-de-Cancer.aspx
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.infocancer.co/portal/#!/filtro_mortalidad/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.datos.gov.co/Salud-y-Protecci-n-Social/Indicadores-mortalidad-y-morbilidad-seg-n-departam/4e4i-ua65/about_data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://geoportal.dane.gov.co/geovisores/sociedad/estadisticas-vitales/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.dane.gov.co/index.php/estadisticas-por-tema/salud/nacimientos-y-defunciones   </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://microdatos.dane.gov.co/index.php/catalog/876/data-dictionary/F35?file_name=nac2023</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.medicinalegal.gov.co/cifras-estadisticas/forensis </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.medicinalegal.gov.co/indicadores-procuraduria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">http://microdatos.dane.gov.co/index.php/catalog/701/get_microdata </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://microdatos.dane.gov.co/index.php/catalog/853/data-dictionary/F1?file_name=Caracteristicas%20generales,%20seguridad%20social%20en%20salud%20y%20educacion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.sispro.gov.co/observatorios/oncancer/Paginas/Observatorio-Nacional-de-Cancer.aspx </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.infocancer.co/portal/#!/filtro_mortalidad/</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Envejecimiento</t>
+  </si>
+  <si>
+    <t>Envejecimiento Poblacional</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2303,6 +2413,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2538,7 +2663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2809,6 +2934,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2819,8 +2947,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3054,6 +3182,428 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A9B6A5-F035-460A-96AE-1565449C8D75}">
+  <sheetPr>
+    <tabColor rgb="FFFF66CC"/>
+  </sheetPr>
+  <dimension ref="A1:T10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" customWidth="1"/>
+    <col min="10" max="10" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="59.21875" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="100"/>
+    </row>
+    <row r="2" spans="1:20" ht="27.6">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="158.4">
+      <c r="A3" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>336</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>519</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="N3" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="T3" s="72"/>
+    </row>
+    <row r="4" spans="1:20" ht="92.4">
+      <c r="A4" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>496</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="L4" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="N4" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="O4" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+    </row>
+    <row r="5" spans="1:20" ht="145.19999999999999">
+      <c r="A5" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>553</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>552</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="61" t="s">
+        <v>555</v>
+      </c>
+      <c r="N5" s="54" t="s">
+        <v>554</v>
+      </c>
+      <c r="O5" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36"/>
+    </row>
+    <row r="6" spans="1:20" ht="92.4">
+      <c r="A6" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>534</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>535</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>536</v>
+      </c>
+      <c r="L6" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>420</v>
+      </c>
+      <c r="N6" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+    </row>
+    <row r="7" spans="1:20" ht="198">
+      <c r="A7" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>537</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>509</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="N7" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="O7" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+    </row>
+    <row r="8" spans="1:20" ht="409.2">
+      <c r="A8" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>410</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>430</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="L8" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>423</v>
+      </c>
+      <c r="N8" s="54" t="s">
+        <v>319</v>
+      </c>
+      <c r="O8" s="36"/>
+      <c r="P8" s="82" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="P10" s="81"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{2F14D376-1E14-483E-8BE9-F0A02468B9A4}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{0ABD05E0-9C1F-4AAA-8CEE-2FE3E788F1DA}"/>
+    <hyperlink ref="J5" r:id="rId3" tooltip="Ministerio de Salud y Protección Social" display="https://www.minsalud.gov.co/" xr:uid="{85434570-94E9-4852-94F7-A7878763A3E9}"/>
+    <hyperlink ref="M5" r:id="rId4" display="https://www.arcgis.com/apps/dashboards/105ba51b48f148f7b4ff21f21ea31b32" xr:uid="{84F4195B-829B-4146-B99E-9E7CADD1F3E3}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{4C4B3A38-24CB-4DB5-A0D9-D3D1B919F51B}"/>
+    <hyperlink ref="M8" r:id="rId6" xr:uid="{5F1C421A-36A4-4068-B2A4-F4A88C81FF13}"/>
+    <hyperlink ref="M7" r:id="rId7" xr:uid="{AC399D3A-B9DC-44D4-A78F-CC1FBDEFC79A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF9900"/>
@@ -3062,7 +3612,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -3077,25 +3627,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:27" ht="41.4">
       <c r="A2" s="1" t="s">
@@ -3138,7 +3688,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
@@ -3188,22 +3738,22 @@
         <v>27</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>198</v>
+        <v>556</v>
       </c>
       <c r="N3" s="83" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>130</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:27" ht="132">
+      <c r="A4" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:27" ht="110.4">
-      <c r="A4" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>188</v>
@@ -3212,10 +3762,10 @@
         <v>189</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>192</v>
@@ -3227,7 +3777,7 @@
         <v>194</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>196</v>
@@ -3238,23 +3788,23 @@
       <c r="L4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>198</v>
+      <c r="M4" s="103" t="s">
+        <v>561</v>
       </c>
       <c r="N4" s="83" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q4" s="8"/>
     </row>
     <row r="5" spans="1:27" ht="345">
       <c r="A5" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>188</v>
@@ -3263,13 +3813,13 @@
         <v>189</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>193</v>
@@ -3278,34 +3828,34 @@
         <v>194</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>196</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N5" s="83" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>130</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q5" s="8"/>
     </row>
     <row r="6" spans="1:27" ht="248.4">
       <c r="A6" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>188</v>
@@ -3314,64 +3864,64 @@
         <v>189</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>437</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>196</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>536</v>
+        <v>557</v>
       </c>
       <c r="N6" s="83" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>130</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q6" s="8"/>
     </row>
     <row r="7" spans="1:27" ht="179.4">
       <c r="A7" s="3" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>188</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>193</v>
@@ -3380,47 +3930,47 @@
         <v>42</v>
       </c>
       <c r="I7" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>228</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:27" ht="138">
       <c r="A8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>188</v>
       </c>
       <c r="C8" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="32" t="s">
         <v>233</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>234</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>193</v>
@@ -3429,28 +3979,28 @@
         <v>42</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J8" s="32" t="s">
         <v>196</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L8" s="32" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="78" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N8" s="84" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="O8" s="32" t="s">
         <v>130</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="12"/>
@@ -3466,22 +4016,22 @@
     </row>
     <row r="9" spans="1:27" ht="132">
       <c r="A9" s="3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>188</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>193</v>
@@ -3490,49 +4040,49 @@
         <v>94</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="L9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="23" t="s">
-        <v>461</v>
+      <c r="M9" s="61" t="s">
+        <v>558</v>
       </c>
       <c r="N9" s="54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O9" s="33" t="s">
         <v>130</v>
       </c>
       <c r="P9" s="56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:27" ht="92.4">
       <c r="A10" s="3" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B10" s="40" t="s">
         <v>188</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>193</v>
@@ -3541,22 +4091,22 @@
         <v>94</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L10" s="33" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N10" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O10" s="33" t="s">
         <v>130</v>
@@ -3566,109 +4116,109 @@
     </row>
     <row r="11" spans="1:27" ht="165.6">
       <c r="A11" s="3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>188</v>
       </c>
       <c r="C11" s="55" t="s">
+        <v>381</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>452</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>453</v>
+      </c>
+      <c r="F11" s="33" t="s">
         <v>382</v>
       </c>
-      <c r="D11" s="55" t="s">
-        <v>456</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>457</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>383</v>
-      </c>
       <c r="G11" s="33" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H11" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L11" s="33" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N11" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O11" s="33" t="s">
         <v>130</v>
       </c>
       <c r="P11" s="21"/>
       <c r="Q11" s="33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="165.6">
       <c r="A12" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>188</v>
       </c>
       <c r="C12" s="55" t="s">
+        <v>384</v>
+      </c>
+      <c r="D12" s="55" t="s">
         <v>385</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="E12" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="G12" s="33" t="s">
         <v>386</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>458</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>383</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>387</v>
       </c>
       <c r="H12" s="33" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N12" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O12" s="33" t="s">
         <v>130</v>
       </c>
       <c r="P12" s="21"/>
       <c r="Q12" s="33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="156">
       <c r="A13" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>188</v>
@@ -3677,13 +4227,13 @@
         <v>189</v>
       </c>
       <c r="D13" s="55" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G13" s="55" t="s">
         <v>193</v>
@@ -3692,22 +4242,22 @@
         <v>42</v>
       </c>
       <c r="I13" s="33" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="L13" s="55" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="N13" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O13" s="33" t="s">
         <v>130</v>
@@ -3717,7 +4267,7 @@
     </row>
     <row r="14" spans="1:27" ht="187.2">
       <c r="A14" s="3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>188</v>
@@ -3726,13 +4276,13 @@
         <v>189</v>
       </c>
       <c r="D14" s="55" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G14" s="55" t="s">
         <v>193</v>
@@ -3741,22 +4291,22 @@
         <v>42</v>
       </c>
       <c r="I14" s="55" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="L14" s="55" t="s">
         <v>27</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="N14" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O14" s="33" t="s">
         <v>130</v>
@@ -3779,12 +4329,13 @@
     <hyperlink ref="M13" r:id="rId7" xr:uid="{1235DFAE-0126-4B6E-AA93-9A6486680F72}"/>
     <hyperlink ref="M14" r:id="rId8" xr:uid="{B0AA7EDD-DC52-45BF-AB92-BE94E52FAFF2}"/>
     <hyperlink ref="M6" r:id="rId9" display="https://www.datos.gov.co/Salud-y-Protecci-n-Social/Razo-n-de-mortalidad-materna-Colombia-y-sus-depart/ck7b-apyq _x000a__x000a_https://geoportal.dane.gov.co/geovisores/sociedad/estadisticas-vitales/" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="M4" r:id="rId10" display="https://www.sispro.gov.co/observatorios/oncancer/Paginas/Observatorio-Nacional-de-Cancer.aspx_x000a__x000a_" xr:uid="{229A1D36-6009-406E-8AD8-42DA8AD3D9C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
@@ -3792,8 +4343,8 @@
   </sheetPr>
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -3812,24 +4363,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="13.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="99"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="100"/>
     </row>
     <row r="2" spans="1:29" ht="27.6">
       <c r="A2" s="1" t="s">
@@ -3869,10 +4420,10 @@
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" s="71" t="s">
         <v>15</v>
@@ -3905,10 +4456,10 @@
         <v>61</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>62</v>
@@ -3931,11 +4482,11 @@
       <c r="L3" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="18" t="s">
-        <v>515</v>
+      <c r="M3" s="103" t="s">
+        <v>559</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>69</v>
@@ -3946,7 +4497,7 @@
     </row>
     <row r="4" spans="1:29" ht="105.6">
       <c r="A4" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>60</v>
@@ -3955,13 +4506,13 @@
         <v>61</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E4" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>277</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>278</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>127</v>
@@ -3970,26 +4521,26 @@
         <v>94</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="L4" s="29" t="s">
         <v>130</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N4" s="29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O4" s="21"/>
       <c r="P4" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="207">
@@ -4003,10 +4554,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>73</v>
@@ -4029,11 +4580,11 @@
       <c r="L5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>515</v>
+      <c r="M5" s="103" t="s">
+        <v>559</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O5" s="6"/>
       <c r="P5" s="6" t="s">
@@ -4054,7 +4605,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>21</v>
@@ -4077,11 +4628,11 @@
       <c r="L6" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="18" t="s">
-        <v>515</v>
+      <c r="M6" s="103" t="s">
+        <v>559</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>81</v>
@@ -4099,13 +4650,13 @@
         <v>83</v>
       </c>
       <c r="D7" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>363</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>364</v>
-      </c>
       <c r="F7" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G7" s="32" t="s">
         <v>63</v>
@@ -4125,11 +4676,11 @@
       <c r="L7" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>515</v>
+      <c r="M7" s="103" t="s">
+        <v>559</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O7" s="32" t="s">
         <v>87</v>
@@ -4143,7 +4694,7 @@
     </row>
     <row r="8" spans="1:29" ht="237.6">
       <c r="A8" s="39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>60</v>
@@ -4152,10 +4703,10 @@
         <v>83</v>
       </c>
       <c r="D8" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>305</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>306</v>
       </c>
       <c r="F8" s="41" t="s">
         <v>21</v>
@@ -4167,25 +4718,25 @@
         <v>94</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N8" s="54" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O8" s="42" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="P8" s="33"/>
       <c r="AC8" s="12"/>
@@ -4201,10 +4752,10 @@
         <v>91</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>92</v>
@@ -4227,18 +4778,18 @@
       <c r="L9" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="M9" s="18" t="s">
-        <v>515</v>
+      <c r="M9" s="103" t="s">
+        <v>559</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O9" s="29"/>
       <c r="P9" s="33"/>
     </row>
     <row r="10" spans="1:29" ht="105.6">
       <c r="A10" s="39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B10" s="43" t="s">
         <v>60</v>
@@ -4247,13 +4798,13 @@
         <v>91</v>
       </c>
       <c r="D10" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="E10" s="29" t="s">
-        <v>303</v>
-      </c>
       <c r="F10" s="25" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G10" s="25" t="s">
         <v>93</v>
@@ -4262,46 +4813,46 @@
         <v>94</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L10" s="33" t="s">
         <v>130</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N10" s="33" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P10" s="33"/>
     </row>
     <row r="11" spans="1:29" ht="79.2">
       <c r="A11" s="57" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B11" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>311</v>
-      </c>
       <c r="E11" s="26" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>127</v>
@@ -4310,44 +4861,44 @@
         <v>94</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="J11" s="42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L11" s="33" t="s">
         <v>130</v>
       </c>
       <c r="M11" s="45" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N11" s="33" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:29" ht="118.8">
       <c r="A12" s="57" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>467</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>322</v>
-      </c>
       <c r="F12" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>93</v>
@@ -4356,44 +4907,44 @@
         <v>94</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>130</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N12" s="33" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="1:29" ht="55.2">
       <c r="A13" s="57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B13" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="D13" s="33" t="s">
         <v>370</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>371</v>
-      </c>
       <c r="E13" s="33" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>127</v>
@@ -4405,13 +4956,13 @@
         <v>94</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K13" s="25" t="s">
         <v>67</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M13" s="33"/>
       <c r="N13" s="33"/>
@@ -4440,7 +4991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -4448,8 +4999,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="D9" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -4465,25 +5016,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="27.6">
       <c r="A2" s="1" t="s">
@@ -4526,7 +5077,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
@@ -4579,7 +5130,7 @@
         <v>140</v>
       </c>
       <c r="N3" s="85" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>130</v>
@@ -4630,7 +5181,7 @@
         <v>146</v>
       </c>
       <c r="N4" s="85" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>130</v>
@@ -4681,7 +5232,7 @@
         <v>154</v>
       </c>
       <c r="N5" s="87" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>130</v>
@@ -4732,7 +5283,7 @@
         <v>154</v>
       </c>
       <c r="N6" s="87" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>130</v>
@@ -4779,11 +5330,11 @@
       <c r="L7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M7" s="18" t="s">
-        <v>517</v>
+      <c r="M7" s="103" t="s">
+        <v>560</v>
       </c>
       <c r="N7" s="85" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>130</v>
@@ -4834,7 +5385,7 @@
         <v>169</v>
       </c>
       <c r="N8" s="85" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>130</v>
@@ -4846,7 +5397,7 @@
     </row>
     <row r="9" spans="1:17" ht="179.4">
       <c r="A9" s="11" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>132</v>
@@ -4882,10 +5433,10 @@
         <v>27</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N9" s="85" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O9" s="6" t="s">
         <v>130</v>
@@ -4903,13 +5454,13 @@
         <v>132</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>21</v>
@@ -4927,16 +5478,16 @@
         <v>138</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N10" s="85" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O10" s="6" t="s">
         <v>130</v>
@@ -4958,16 +5509,16 @@
     <hyperlink ref="M4" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
     <hyperlink ref="M5" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
     <hyperlink ref="M6" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="M7" r:id="rId5" display="http://microdatos.dane.gov.co/index.php/catalog/701/get_microdata" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="M8" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="M9" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="M10" r:id="rId8" xr:uid="{9017CF82-9B1F-4582-88E8-9F21BEB1DE20}"/>
+    <hyperlink ref="M8" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="M9" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="M10" r:id="rId7" xr:uid="{9017CF82-9B1F-4582-88E8-9F21BEB1DE20}"/>
+    <hyperlink ref="M7" r:id="rId8" display="http://microdatos.dane.gov.co/index.php/catalog/701/get_microdata" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF993366"/>
@@ -4975,7 +5526,7 @@
   </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -4992,25 +5543,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="41.4">
       <c r="A2" s="1" t="s">
@@ -5053,7 +5604,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
@@ -5079,7 +5630,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>100</v>
@@ -5148,10 +5699,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="N4" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>105</v>
@@ -5199,16 +5750,16 @@
         <v>27</v>
       </c>
       <c r="M5" s="58" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="N5" s="66" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O5" s="32" t="s">
         <v>119</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="Q5" s="35"/>
     </row>
@@ -5226,7 +5777,7 @@
         <v>122</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>21</v>
@@ -5238,7 +5789,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="J6" s="33" t="s">
         <v>112</v>
@@ -5250,10 +5801,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="23" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="N6" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O6" s="33" t="s">
         <v>119</v>
@@ -5265,7 +5816,7 @@
     </row>
     <row r="7" spans="1:17" ht="234.6">
       <c r="A7" s="43" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="B7" s="43" t="s">
         <v>97</v>
@@ -5274,10 +5825,10 @@
         <v>108</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="F7" s="33" t="s">
         <v>21</v>
@@ -5289,7 +5840,7 @@
         <v>42</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="J7" s="33" t="s">
         <v>112</v>
@@ -5301,16 +5852,16 @@
         <v>27</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O7" s="33" t="s">
         <v>119</v>
       </c>
       <c r="P7" s="33" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="Q7" s="36"/>
     </row>
@@ -5328,7 +5879,7 @@
         <v>125</v>
       </c>
       <c r="E8" s="90" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="F8" s="90" t="s">
         <v>126</v>
@@ -5359,19 +5910,19 @@
     </row>
     <row r="9" spans="1:17" ht="105.6">
       <c r="A9" s="43" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B9" s="43" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="F9" s="33" t="s">
         <v>21</v>
@@ -5383,22 +5934,22 @@
         <v>42</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="L9" s="26" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O9" s="93" t="s">
         <v>130</v>
@@ -5425,7 +5976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -5434,7 +5985,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -5450,25 +6001,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="27.6">
       <c r="A2" s="1" t="s">
@@ -5511,7 +6062,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>14</v>
@@ -5537,7 +6088,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>21</v>
@@ -5561,7 +6112,7 @@
         <v>27</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="6" t="s">
@@ -5586,10 +6137,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>22</v>
@@ -5674,7 +6225,7 @@
     </row>
     <row r="6" spans="1:17" ht="179.4">
       <c r="A6" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -5710,7 +6261,7 @@
         <v>27</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N6" s="58"/>
       <c r="O6" s="6" t="s">
@@ -5723,7 +6274,7 @@
     </row>
     <row r="7" spans="1:17" ht="331.2">
       <c r="A7" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>45</v>
@@ -5759,7 +6310,7 @@
         <v>27</v>
       </c>
       <c r="M7" s="64" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="60" t="s">
@@ -5772,7 +6323,7 @@
     </row>
     <row r="8" spans="1:17" ht="224.4">
       <c r="A8" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>45</v>
@@ -5808,7 +6359,7 @@
         <v>27</v>
       </c>
       <c r="M8" s="61" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N8" s="61"/>
       <c r="O8" s="33" t="s">
@@ -5827,25 +6378,25 @@
         <v>18</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="F9" s="36" t="s">
         <v>332</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>331</v>
-      </c>
-      <c r="F9" s="36" t="s">
+      <c r="G9" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="G9" s="26" t="s">
-        <v>334</v>
-      </c>
       <c r="H9" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>25</v>
@@ -5857,54 +6408,54 @@
         <v>27</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
     </row>
     <row r="10" spans="1:17" ht="145.19999999999999">
       <c r="A10" s="4" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B10" s="43" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D10" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F10" s="36" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="H10" s="26" t="s">
-        <v>343</v>
-      </c>
       <c r="I10" s="25" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="J10" s="37" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="36" t="s">
@@ -5921,13 +6472,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E11" s="66" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>21</v>
@@ -5936,22 +6487,22 @@
         <v>93</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I11" s="80" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="J11" s="68" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L11" s="67" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="70" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N11" s="70"/>
       <c r="O11" s="67" t="s">
@@ -5962,49 +6513,49 @@
     </row>
     <row r="12" spans="1:17" ht="118.8">
       <c r="A12" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D12" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>399</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>400</v>
       </c>
       <c r="F12" s="36" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="J12" s="37" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L12" s="36" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N12" s="36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O12" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
@@ -6391,7 +6942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF6600CC"/>
@@ -6399,7 +6950,7 @@
   </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -6415,25 +6966,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="41.4">
       <c r="A2" s="1" t="s">
@@ -6476,7 +7027,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O2" s="49" t="s">
         <v>14</v>
@@ -6490,22 +7041,22 @@
     </row>
     <row r="3" spans="1:17" ht="110.4">
       <c r="A3" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>193</v>
@@ -6514,47 +7065,47 @@
         <v>42</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N3" s="53"/>
       <c r="O3" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17" ht="96.6">
       <c r="A4" s="4" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>193</v>
@@ -6563,47 +7114,47 @@
         <v>94</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="79" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N4" s="53"/>
       <c r="O4" s="28" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="1:17" ht="110.4">
       <c r="A5" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>251</v>
-      </c>
       <c r="D5" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="20" t="s">
         <v>262</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>263</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>193</v>
@@ -6612,47 +7163,47 @@
         <v>94</v>
       </c>
       <c r="I5" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="K5" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="M5" s="47" t="s">
         <v>265</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="M5" s="47" t="s">
-        <v>266</v>
       </c>
       <c r="N5" s="25"/>
       <c r="O5" s="50" t="s">
         <v>130</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:17" ht="105.6">
       <c r="A6" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C6" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>280</v>
       </c>
       <c r="G6" s="28" t="s">
         <v>193</v>
@@ -6661,49 +7212,49 @@
         <v>94</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="L6" s="24" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N6" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O6" s="50" t="s">
         <v>130</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="1:17" ht="105.6">
       <c r="A7" s="4" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G7" s="28" t="s">
         <v>193</v>
@@ -6712,49 +7263,49 @@
         <v>94</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N7" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O7" s="50" t="s">
         <v>130</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:17" ht="132">
       <c r="A8" s="4" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G8" s="24" t="s">
         <v>193</v>
@@ -6763,42 +7314,42 @@
         <v>94</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="24" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N8" s="54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O8" s="51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="P8" s="21"/>
       <c r="Q8" s="26"/>
     </row>
     <row r="9" spans="1:17" ht="69">
       <c r="A9" s="4" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F9" s="26" t="s">
         <v>21</v>
@@ -6810,45 +7361,45 @@
         <v>94</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="24" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="N9" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="O9" s="51" t="s">
         <v>290</v>
-      </c>
-      <c r="N9" s="54" t="s">
-        <v>318</v>
-      </c>
-      <c r="O9" s="51" t="s">
-        <v>291</v>
       </c>
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:17" ht="118.8">
       <c r="A10" s="4" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C10" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="E10" s="26" t="s">
         <v>376</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="F10" s="26" t="s">
         <v>377</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>378</v>
       </c>
       <c r="G10" s="24" t="s">
         <v>193</v>
@@ -6857,25 +7408,25 @@
         <v>94</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="J10" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="K10" s="25" t="s">
         <v>379</v>
-      </c>
-      <c r="K10" s="25" t="s">
-        <v>380</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N10" s="62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O10" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
@@ -6899,14 +7450,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F58EE5F-4C67-4F95-A4D6-99AEBFC15EE8}">
   <sheetPr>
     <tabColor rgb="FF996600"/>
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -6969,7 +7520,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O1" s="77" t="s">
         <v>14</v>
@@ -6982,20 +7533,20 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="145.19999999999999">
-      <c r="A2" s="102" t="s">
-        <v>557</v>
+      <c r="A2" s="96" t="s">
+        <v>549</v>
       </c>
       <c r="B2" s="63" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="63" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="D2" s="29" t="s">
         <v>389</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>390</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>391</v>
       </c>
       <c r="F2" s="63" t="s">
         <v>21</v>
@@ -7004,77 +7555,77 @@
         <v>193</v>
       </c>
       <c r="H2" s="63" t="s">
+        <v>391</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>551</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>392</v>
       </c>
-      <c r="I2" s="29" t="s">
-        <v>559</v>
-      </c>
-      <c r="J2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>393</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>394</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="M2" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="N2" s="26" t="s">
         <v>396</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>397</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>398</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
     </row>
     <row r="3" spans="1:17" ht="171.6">
       <c r="A3" s="63" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="F3" s="63" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H3" s="63" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M3" s="23" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="O3" s="63" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
@@ -7238,424 +7789,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A9B6A5-F035-460A-96AE-1565449C8D75}">
-  <sheetPr>
-    <tabColor rgb="FFFF66CC"/>
-  </sheetPr>
-  <dimension ref="A1:T10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
-  <cols>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.109375" customWidth="1"/>
-    <col min="10" max="10" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="59.21875" customWidth="1"/>
-    <col min="17" max="17" width="30.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="99"/>
-    </row>
-    <row r="2" spans="1:20" ht="27.6">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="52" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="158.4">
-      <c r="A3" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>522</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>523</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>521</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>275</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>526</v>
-      </c>
-      <c r="J3" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>338</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="N3" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="T3" s="72"/>
-    </row>
-    <row r="4" spans="1:20" ht="92.4">
-      <c r="A4" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>520</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>416</v>
-      </c>
-      <c r="G4" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="I4" s="33" t="s">
-        <v>501</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>338</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="N4" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="O4" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-    </row>
-    <row r="5" spans="1:20" ht="145.19999999999999">
-      <c r="A5" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>419</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>502</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="K5" s="25" t="s">
-        <v>560</v>
-      </c>
-      <c r="L5" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="23" t="s">
-        <v>421</v>
-      </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
-    </row>
-    <row r="6" spans="1:20" ht="92.4">
-      <c r="A6" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>540</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>539</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>541</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>542</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>543</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>544</v>
-      </c>
-      <c r="L6" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="23" t="s">
-        <v>424</v>
-      </c>
-      <c r="N6" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="O6" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-    </row>
-    <row r="7" spans="1:20" ht="198">
-      <c r="A7" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>545</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>514</v>
-      </c>
-      <c r="L7" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="N7" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="O7" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-    </row>
-    <row r="8" spans="1:20" ht="409.2">
-      <c r="A8" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>411</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>428</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>434</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>503</v>
-      </c>
-      <c r="J8" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>427</v>
-      </c>
-      <c r="N8" s="54" t="s">
-        <v>320</v>
-      </c>
-      <c r="O8" s="36"/>
-      <c r="P8" s="82" t="s">
-        <v>504</v>
-      </c>
-      <c r="Q8" s="26" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="P10" s="81"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Q1"/>
-  </mergeCells>
-  <phoneticPr fontId="22" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{2F14D376-1E14-483E-8BE9-F0A02468B9A4}"/>
-    <hyperlink ref="M4" r:id="rId2" xr:uid="{0ABD05E0-9C1F-4AAA-8CEE-2FE3E788F1DA}"/>
-    <hyperlink ref="J5" r:id="rId3" tooltip="Ministerio de Salud y Protección Social" display="https://www.minsalud.gov.co/" xr:uid="{85434570-94E9-4852-94F7-A7878763A3E9}"/>
-    <hyperlink ref="M5" r:id="rId4" xr:uid="{84F4195B-829B-4146-B99E-9E7CADD1F3E3}"/>
-    <hyperlink ref="M6" r:id="rId5" xr:uid="{4C4B3A38-24CB-4DB5-A0D9-D3D1B919F51B}"/>
-    <hyperlink ref="M8" r:id="rId6" xr:uid="{5F1C421A-36A4-4068-B2A4-F4A88C81FF13}"/>
-    <hyperlink ref="M7" r:id="rId7" xr:uid="{AC399D3A-B9DC-44D4-A78F-CC1FBDEFC79A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se realizo ajuste a Cauca_Bateria de indicadores V1
</commit_message>
<xml_diff>
--- a/data/Cauca_Bateria de indicadores V1 .xlsx
+++ b/data/Cauca_Bateria de indicadores V1 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\observatorio-mujer-cauca\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732CF4F9-5C92-4228-B704-ED23684D7568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F468F1-43D5-4FC9-81E0-35FA8D26B233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sociodemografico" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="558">
   <si>
     <t>Bateria de indicadores OBSERVATORIO DE ASUNTOS DE LAS MUJERES DEL DEPARTAMENTO DEL CAUCA</t>
   </si>
@@ -1162,24 +1162,6 @@
     <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/salud/calidad-de-vida-ecv/encuesta-nacional-de-calidad-de-vida-ecv-2024</t>
   </si>
   <si>
-    <t>Trabajo doméstico y de cuidados no remunerado</t>
-  </si>
-  <si>
-    <t>Medir la distribución del tiempo que mujeres y hombres dedican diariamente al trabajo doméstico y de cuidados no remunerado, con el fin de visibilizar las desigualdades de género en la carga de trabajo no remunerado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional, grupo etario </t>
-  </si>
-  <si>
-    <t>Horas promedio diarias</t>
-  </si>
-  <si>
-    <t>Encuesta Nacional de Uso del Tiempo (ENUT)</t>
-  </si>
-  <si>
-    <t>https://www.dane.gov.co/index.php/estadisticas-por-tema/pobreza-y-condiciones-de-vida/encuesta-nacional-del-uso-del-tiempo-enut</t>
-  </si>
-  <si>
     <t>Dinámicas de empobrecimiento</t>
   </si>
   <si>
@@ -1195,9 +1177,6 @@
     <t>AE06</t>
   </si>
   <si>
-    <t>AE10</t>
-  </si>
-  <si>
     <t>VBG01</t>
   </si>
   <si>
@@ -1604,9 +1583,6 @@
   </si>
   <si>
     <t>(Numero de jovenes desocupados de 14–28 años en Popayan/Poblacion economicamente activa (ocupados + desocupados) de 14–28 años en Popayan)×100</t>
-  </si>
-  <si>
-    <t>(Total de horas diarias reportadas en trabajo domestico y de cuidados no remunerado por las personas de un sexo/Numero total de personas de ese sexo encuestadas)</t>
   </si>
   <si>
     <t>(Numero de personas que pasan de no pobres a pobres entre t−1 y t/Numero total de personas que no eran pobres en t−1)×100</t>
@@ -1850,33 +1826,6 @@
         <scheme val="major"/>
       </rPr>
       <t xml:space="preserve"> para contexto.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">https://www.dane.gov.co/index.php/estadisticas-por-tema/cuentas-nacionales/cuentas-satelite/cuentas-economicas-cuenta-satelite-economia-del-cuidado       </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="7"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> https://microdatos.dane.gov.co/index.php/catalog/729         </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color theme="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                                                                                                                                                                                            </t>
     </r>
   </si>
   <si>
@@ -2231,12 +2180,67 @@
       <t>https://microdatos.dane.gov.co/index.php/catalog/876/data-dictionary/F35?file_name=nac2023</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.dane.gov.co/index.php/estadisticas-por-tema/cuentas-nacionales/cuentas-satelite/cuentas-economicas-cuenta-satelite-economia-del-cuidado       </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> https://microdatos.dane.gov.co/index.php/catalog/729    </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">https://www.dane.gov.co/index.php/estadisticas-por-tema/pobreza-y-condiciones-de-vida/encuesta-nacional-del-uso-del-tiempo-enut  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="7"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                                                                                                                                                                            </t>
+    </r>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>XLS, CSV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2424,6 +2428,14 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -2690,7 +2702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2901,7 +2913,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2913,52 +2925,55 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3195,7 +3210,7 @@
   </sheetPr>
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -3217,94 +3232,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="84" t="s">
+      <c r="N2" s="81" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="93" t="s">
+      <c r="Q2" s="85" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="158.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="F3" s="29" t="s">
         <v>332</v>
@@ -3316,7 +3331,7 @@
         <v>274</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>25</v>
@@ -3342,31 +3357,31 @@
     </row>
     <row r="4" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>25</v>
@@ -3391,19 +3406,19 @@
     </row>
     <row r="5" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>405</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>546</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>547</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>412</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>21</v>
@@ -3412,25 +3427,25 @@
         <v>93</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="L5" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="O5" s="31" t="s">
         <v>28</v>
@@ -3438,45 +3453,45 @@
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
     </row>
-    <row r="6" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="L6" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="N6" s="48" t="s">
         <v>315</v>
@@ -3487,21 +3502,21 @@
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
     </row>
-    <row r="7" spans="1:20" ht="198" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -3510,16 +3525,16 @@
         <v>93</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="L7" s="31" t="s">
         <v>27</v>
@@ -3538,19 +3553,19 @@
     </row>
     <row r="8" spans="1:20" ht="409.2" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>21</v>
@@ -3559,32 +3574,32 @@
         <v>93</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="L8" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="N8" s="48" t="s">
         <v>315</v>
       </c>
       <c r="O8" s="31"/>
       <c r="P8" s="12" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3637,76 +3652,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="85" t="s">
+      <c r="N2" s="82" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="84" t="s">
+      <c r="P2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="84" t="s">
+      <c r="Q2" s="81" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3748,10 +3763,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="63" t="s">
-        <v>560</v>
-      </c>
-      <c r="N3" s="95" t="s">
-        <v>520</v>
+        <v>551</v>
+      </c>
+      <c r="N3" s="87" t="s">
+        <v>512</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>130</v>
@@ -3799,10 +3814,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>561</v>
-      </c>
-      <c r="N4" s="95" t="s">
-        <v>520</v>
+        <v>552</v>
+      </c>
+      <c r="N4" s="87" t="s">
+        <v>512</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>130</v>
@@ -3826,7 +3841,7 @@
         <v>204</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>205</v>
@@ -3852,8 +3867,8 @@
       <c r="M5" s="63" t="s">
         <v>208</v>
       </c>
-      <c r="N5" s="95" t="s">
-        <v>520</v>
+      <c r="N5" s="87" t="s">
+        <v>512</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
@@ -3877,7 +3892,7 @@
         <v>211</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>212</v>
@@ -3900,11 +3915,11 @@
       <c r="L6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="96" t="s">
-        <v>562</v>
-      </c>
-      <c r="N6" s="95" t="s">
-        <v>521</v>
+      <c r="M6" s="88" t="s">
+        <v>553</v>
+      </c>
+      <c r="N6" s="87" t="s">
+        <v>513</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
@@ -3916,7 +3931,7 @@
     </row>
     <row r="7" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>188</v>
@@ -4000,11 +4015,11 @@
       <c r="L8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="97" t="s">
+      <c r="M8" s="89" t="s">
         <v>236</v>
       </c>
-      <c r="N8" s="98" t="s">
-        <v>522</v>
+      <c r="N8" s="90" t="s">
+        <v>514</v>
       </c>
       <c r="O8" s="27" t="s">
         <v>130</v>
@@ -4026,19 +4041,19 @@
     </row>
     <row r="9" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B9" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="91" t="s">
         <v>270</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>269</v>
@@ -4050,19 +4065,19 @@
         <v>94</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>310</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="L9" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="N9" s="48" t="s">
         <v>313</v>
@@ -4077,22 +4092,22 @@
     </row>
     <row r="10" spans="1:27" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="91" t="s">
         <v>311</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>193</v>
@@ -4101,19 +4116,19 @@
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="J10" s="14" t="s">
         <v>310</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="L10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="N10" s="48" t="s">
         <v>315</v>
@@ -4126,43 +4141,43 @@
     </row>
     <row r="11" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B11" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="99" t="s">
-        <v>376</v>
-      </c>
-      <c r="D11" s="99" t="s">
-        <v>447</v>
+      <c r="C11" s="91" t="s">
+        <v>369</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>440</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>310</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="L11" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="N11" s="48" t="s">
         <v>315</v>
@@ -4172,48 +4187,48 @@
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="29" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B12" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="99" t="s">
-        <v>379</v>
-      </c>
-      <c r="D12" s="99" t="s">
-        <v>380</v>
+      <c r="C12" s="91" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>373</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>310</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="L12" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="N12" s="48" t="s">
         <v>315</v>
@@ -4223,48 +4238,48 @@
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="29" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="91" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="99" t="s">
-        <v>440</v>
-      </c>
-      <c r="E13" s="99" t="s">
-        <v>450</v>
-      </c>
-      <c r="F13" s="99" t="s">
-        <v>441</v>
-      </c>
-      <c r="G13" s="99" t="s">
+      <c r="D13" s="91" t="s">
+        <v>433</v>
+      </c>
+      <c r="E13" s="91" t="s">
+        <v>443</v>
+      </c>
+      <c r="F13" s="91" t="s">
+        <v>434</v>
+      </c>
+      <c r="G13" s="91" t="s">
         <v>193</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="L13" s="99" t="s">
+        <v>432</v>
+      </c>
+      <c r="L13" s="91" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="N13" s="48" t="s">
         <v>315</v>
@@ -4272,48 +4287,48 @@
       <c r="O13" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="99"/>
+      <c r="P13" s="91"/>
+      <c r="Q13" s="91"/>
     </row>
     <row r="14" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B14" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="91" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="99" t="s">
-        <v>451</v>
-      </c>
-      <c r="E14" s="99" t="s">
-        <v>436</v>
-      </c>
-      <c r="F14" s="99" t="s">
-        <v>437</v>
-      </c>
-      <c r="G14" s="99" t="s">
+      <c r="D14" s="91" t="s">
+        <v>444</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>429</v>
+      </c>
+      <c r="F14" s="91" t="s">
+        <v>430</v>
+      </c>
+      <c r="G14" s="91" t="s">
         <v>193</v>
       </c>
-      <c r="H14" s="99" t="s">
+      <c r="H14" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="99" t="s">
-        <v>473</v>
+      <c r="I14" s="91" t="s">
+        <v>466</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="L14" s="99" t="s">
+        <v>432</v>
+      </c>
+      <c r="L14" s="91" t="s">
         <v>27</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="N14" s="48" t="s">
         <v>315</v>
@@ -4321,8 +4336,8 @@
       <c r="O14" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P14" s="99"/>
-      <c r="Q14" s="99"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4373,76 +4388,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:30" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="84" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="82" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="84" t="s">
+      <c r="N2" s="81" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="86" t="s">
+      <c r="Q2" s="80" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="2"/>
@@ -4470,10 +4485,10 @@
         <v>61</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>62</v>
@@ -4497,7 +4512,7 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>315</v>
@@ -4523,7 +4538,7 @@
         <v>61</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>276</v>
@@ -4538,13 +4553,13 @@
         <v>94</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>27</v>
@@ -4560,7 +4575,7 @@
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="14" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="211.2" x14ac:dyDescent="0.25">
@@ -4574,10 +4589,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>73</v>
@@ -4601,7 +4616,7 @@
         <v>27</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="N5" s="18" t="s">
         <v>315</v>
@@ -4628,7 +4643,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>21</v>
@@ -4652,7 +4667,7 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="N6" s="19" t="s">
         <v>315</v>
@@ -4676,10 +4691,10 @@
         <v>83</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>268</v>
@@ -4703,7 +4718,7 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="N7" s="27" t="s">
         <v>315</v>
@@ -4747,13 +4762,13 @@
         <v>94</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="J8" s="29" t="s">
         <v>303</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>27</v>
@@ -4762,7 +4777,7 @@
         <v>305</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="O8" s="29" t="s">
         <v>247</v>
@@ -4784,10 +4799,10 @@
         <v>91</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>92</v>
@@ -4811,7 +4826,7 @@
         <v>27</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="N9" s="29" t="s">
         <v>315</v>
@@ -4839,7 +4854,7 @@
         <v>299</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>93</v>
@@ -4848,10 +4863,10 @@
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>300</v>
@@ -4863,7 +4878,7 @@
         <v>319</v>
       </c>
       <c r="N10" s="29" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>130</v>
@@ -4881,13 +4896,13 @@
         <v>60</v>
       </c>
       <c r="C11" s="72" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>306</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>205</v>
@@ -4899,13 +4914,13 @@
         <v>94</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="J11" s="71" t="s">
         <v>308</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="L11" s="18" t="s">
         <v>27</v>
@@ -4914,7 +4929,7 @@
         <v>309</v>
       </c>
       <c r="N11" s="29" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="O11" s="29" t="s">
         <v>130</v>
@@ -4924,7 +4939,7 @@
     </row>
     <row r="12" spans="1:30" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>60</v>
@@ -4933,7 +4948,7 @@
         <v>316</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>317</v>
@@ -4948,13 +4963,13 @@
         <v>94</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="J12" s="71" t="s">
         <v>308</v>
       </c>
       <c r="K12" s="71" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="L12" s="18" t="s">
         <v>27</v>
@@ -4963,7 +4978,7 @@
         <v>318</v>
       </c>
       <c r="N12" s="29" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="O12" s="29" t="s">
         <v>130</v>
@@ -4973,16 +4988,16 @@
     </row>
     <row r="13" spans="1:30" ht="66" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>275</v>
@@ -5063,76 +5078,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
-    </row>
-    <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="97"/>
+    </row>
+    <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="84" t="s">
+      <c r="N2" s="81" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="84" t="s">
+      <c r="P2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="84" t="s">
+      <c r="Q2" s="81" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5279,7 +5294,7 @@
         <v>154</v>
       </c>
       <c r="N5" s="62" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
@@ -5330,7 +5345,7 @@
         <v>154</v>
       </c>
       <c r="N6" s="62" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
@@ -5378,10 +5393,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="N7" s="60" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="O7" s="19" t="s">
         <v>130</v>
@@ -5432,7 +5447,7 @@
         <v>169</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="O8" s="19" t="s">
         <v>130</v>
@@ -5444,7 +5459,7 @@
     </row>
     <row r="9" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>132</v>
@@ -5501,13 +5516,13 @@
         <v>132</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>21</v>
@@ -5525,13 +5540,13 @@
         <v>138</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="N10" s="60" t="s">
         <v>315</v>
@@ -5591,76 +5606,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="84" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="M2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="84" t="s">
-        <v>348</v>
-      </c>
-      <c r="O2" s="85" t="s">
+      <c r="N2" s="81" t="s">
+        <v>341</v>
+      </c>
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="84" t="s">
+      <c r="P2" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="84" t="s">
+      <c r="Q2" s="81" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5678,7 +5693,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>100</v>
@@ -5747,10 +5762,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>105</v>
@@ -5798,16 +5813,16 @@
         <v>27</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>119</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="Q5" s="30"/>
     </row>
@@ -5825,7 +5840,7 @@
         <v>122</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>21</v>
@@ -5837,7 +5852,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="J6" s="29" t="s">
         <v>112</v>
@@ -5849,10 +5864,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>119</v>
@@ -5864,7 +5879,7 @@
     </row>
     <row r="7" spans="1:17" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>97</v>
@@ -5873,10 +5888,10 @@
         <v>108</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -5888,7 +5903,7 @@
         <v>42</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="J7" s="29" t="s">
         <v>112</v>
@@ -5900,16 +5915,16 @@
         <v>27</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="O7" s="29" t="s">
         <v>119</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="Q7" s="31"/>
     </row>
@@ -5927,7 +5942,7 @@
         <v>125</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>126</v>
@@ -5958,19 +5973,19 @@
     </row>
     <row r="9" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>21</v>
@@ -5982,19 +5997,19 @@
         <v>42</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>315</v>
@@ -6030,10 +6045,10 @@
     <tabColor rgb="FF00B0F0"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6044,84 +6059,84 @@
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="10" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="37.109375" customWidth="1"/>
     <col min="17" max="17" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="89"/>
-    </row>
-    <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="95"/>
+    </row>
+    <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="84" t="s">
+      <c r="N2" s="81" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="90" t="s">
+      <c r="P2" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="90" t="s">
+      <c r="Q2" s="83" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6139,7 +6154,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>21</v>
@@ -6163,9 +6178,11 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>351</v>
-      </c>
-      <c r="N3" s="20"/>
+        <v>344</v>
+      </c>
+      <c r="N3" s="60" t="s">
+        <v>315</v>
+      </c>
       <c r="O3" s="19" t="s">
         <v>28</v>
       </c>
@@ -6188,7 +6205,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>267</v>
@@ -6214,7 +6231,9 @@
       <c r="M4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="20"/>
+      <c r="N4" s="60" t="s">
+        <v>315</v>
+      </c>
       <c r="O4" s="19" t="s">
         <v>28</v>
       </c>
@@ -6265,7 +6284,9 @@
       <c r="M5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="20"/>
+      <c r="N5" s="60" t="s">
+        <v>315</v>
+      </c>
       <c r="O5" s="19" t="s">
         <v>28</v>
       </c>
@@ -6276,7 +6297,7 @@
     </row>
     <row r="6" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>18</v>
@@ -6312,9 +6333,11 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="N6" s="23"/>
+        <v>343</v>
+      </c>
+      <c r="N6" s="100" t="s">
+        <v>556</v>
+      </c>
       <c r="O6" s="19" t="s">
         <v>28</v>
       </c>
@@ -6325,7 +6348,7 @@
     </row>
     <row r="7" spans="1:17" ht="343.2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>45</v>
@@ -6361,9 +6384,11 @@
         <v>27</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="N7" s="15"/>
+        <v>343</v>
+      </c>
+      <c r="N7" s="100" t="s">
+        <v>556</v>
+      </c>
       <c r="O7" s="25" t="s">
         <v>28</v>
       </c>
@@ -6372,9 +6397,9 @@
       </c>
       <c r="Q7" s="21"/>
     </row>
-    <row r="8" spans="1:17" ht="224.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="369.6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>45</v>
@@ -6410,9 +6435,11 @@
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>549</v>
-      </c>
-      <c r="N8" s="15"/>
+        <v>555</v>
+      </c>
+      <c r="N8" s="48" t="s">
+        <v>557</v>
+      </c>
       <c r="O8" s="29" t="s">
         <v>28</v>
       </c>
@@ -6447,7 +6474,7 @@
         <v>274</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>25</v>
@@ -6461,155 +6488,131 @@
       <c r="M9" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="48" t="s">
+        <v>315</v>
+      </c>
       <c r="O9" s="29" t="s">
         <v>331</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
     </row>
-    <row r="10" spans="1:17" ht="145.19999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>464</v>
-      </c>
-      <c r="B10" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="B10" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="F10" s="31" t="s">
+      <c r="D10" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>458</v>
+      </c>
+      <c r="F10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>337</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>483</v>
-      </c>
-      <c r="J10" s="13" t="s">
+      <c r="G10" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>476</v>
+      </c>
+      <c r="J10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="L10" s="31" t="s">
+      <c r="K10" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="L10" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="31" t="s">
+      <c r="M10" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="N10" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="O10" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-    </row>
-    <row r="11" spans="1:17" ht="132" x14ac:dyDescent="0.25">
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+    </row>
+    <row r="11" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>352</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>465</v>
-      </c>
-      <c r="F11" s="34" t="s">
+      <c r="C11" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="34" t="s">
+      <c r="G11" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="I11" s="35" t="s">
-        <v>484</v>
-      </c>
-      <c r="J11" s="36" t="s">
+      <c r="I11" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="33" t="s">
-        <v>333</v>
-      </c>
-      <c r="L11" s="34" t="s">
+      <c r="K11" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="L11" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="37" t="s">
-        <v>334</v>
-      </c>
-      <c r="N11" s="37"/>
-      <c r="O11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-    </row>
-    <row r="12" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>404</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>274</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>485</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="L12" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="N12" s="31" t="s">
+      <c r="M11" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="N11" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="O12" s="31" t="s">
+      <c r="O11" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+    </row>
+    <row r="12" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -6953,25 +6956,6 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>
@@ -6984,10 +6968,9 @@
     <hyperlink ref="M6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="M8" r:id="rId5" display="https://www.dane.gov.co/index.php/estadisticas-por-tema/cuentas-nacionales/cuentas-satelite/cuentas-economicas-cuenta-satelite-economia-del-cuidado                                                                                                                                                                                                                                                                                                                             " xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="M9" r:id="rId6" xr:uid="{DC631C5E-16D4-41B7-9049-12D0D8C2A754}"/>
-    <hyperlink ref="M10" r:id="rId7" xr:uid="{E97D0C11-978A-4F67-961E-8A1029E45BC6}"/>
-    <hyperlink ref="M11" r:id="rId8" xr:uid="{ECC4F51B-C5FA-439D-A796-88212E18B19E}"/>
-    <hyperlink ref="M7" r:id="rId9" xr:uid="{BFBAEAB1-4A71-430D-931D-80EE25B7648E}"/>
-    <hyperlink ref="M12" r:id="rId10" xr:uid="{ABA6DC79-74FD-476A-BB89-BB309BA006D0}"/>
+    <hyperlink ref="M10" r:id="rId7" xr:uid="{ECC4F51B-C5FA-439D-A796-88212E18B19E}"/>
+    <hyperlink ref="M7" r:id="rId8" xr:uid="{BFBAEAB1-4A71-430D-931D-80EE25B7648E}"/>
+    <hyperlink ref="M11" r:id="rId9" xr:uid="{ABA6DC79-74FD-476A-BB89-BB309BA006D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7020,76 +7003,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="89"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="92" t="s">
+      <c r="M2" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="93" t="s">
+      <c r="N2" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="O2" s="94" t="s">
+      <c r="O2" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="90" t="s">
+      <c r="P2" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="90" t="s">
+      <c r="Q2" s="83" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7098,7 +7081,7 @@
         <v>238</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>239</v>
@@ -7144,10 +7127,10 @@
     </row>
     <row r="4" spans="1:17" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>250</v>
@@ -7196,7 +7179,7 @@
         <v>249</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>250</v>
@@ -7245,7 +7228,7 @@
         <v>259</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>278</v>
@@ -7266,13 +7249,13 @@
         <v>94</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="L6" s="46" t="s">
         <v>27</v>
@@ -7287,16 +7270,16 @@
         <v>130</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>281</v>
@@ -7317,13 +7300,13 @@
         <v>94</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="J7" s="49" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="L7" s="46" t="s">
         <v>27</v>
@@ -7338,16 +7321,16 @@
         <v>130</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>282</v>
@@ -7368,7 +7351,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>283</v>
@@ -7391,10 +7374,10 @@
     </row>
     <row r="9" spans="1:17" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>285</v>
@@ -7415,7 +7398,7 @@
         <v>94</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>283</v>
@@ -7438,22 +7421,22 @@
     </row>
     <row r="10" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="G10" s="46" t="s">
         <v>193</v>
@@ -7462,19 +7445,19 @@
         <v>94</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="L10" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="N10" s="51" t="s">
         <v>315</v>
@@ -7534,25 +7517,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
@@ -7609,19 +7592,19 @@
     </row>
     <row r="3" spans="1:17" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>21</v>
@@ -7630,77 +7613,77 @@
         <v>193</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>

</xml_diff>

<commit_message>
Se realizo ajuste de la bateria de indicadores en base a las correcciones sugeridas
</commit_message>
<xml_diff>
--- a/data/Cauca_Bateria de indicadores V1 .xlsx
+++ b/data/Cauca_Bateria de indicadores V1 .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\observatorio-mujer-cauca\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F468F1-43D5-4FC9-81E0-35FA8D26B233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1DD80C-0861-457F-85C3-DCB7CE1B8FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sociodemografico" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="541">
   <si>
     <t>Bateria de indicadores OBSERVATORIO DE ASUNTOS DE LAS MUJERES DEL DEPARTAMENTO DEL CAUCA</t>
   </si>
@@ -1051,30 +1051,6 @@
     <t>Enlace</t>
   </si>
   <si>
-    <t>Casos de feminicidio registrados en el dpto. del Cauca</t>
-  </si>
-  <si>
-    <t>Medir la magnitud de los feminicidios en el dpto. del Cauca para visibilizar la violencia letal contra las mujeres y aportar a la formulación de políticas públicas de prevención y sanción.</t>
-  </si>
-  <si>
-    <t>Observatorio Colombiano de Feminicidios</t>
-  </si>
-  <si>
-    <t>Tasa de homicidios por género en el departamento del Cauca</t>
-  </si>
-  <si>
-    <t>Medir la magnitud de los homicidios en el dpto. del Cauca, diferenciados por sexo y grupo etario, para identificar poblaciones más vulnerables y orientar políticas de prevención.</t>
-  </si>
-  <si>
-    <t>Ministerio de Justicia y del Derecho</t>
-  </si>
-  <si>
-    <t>​​</t>
-  </si>
-  <si>
-    <t>https://www.minjusticia.gov.co/programas-co/politica-criminal/Paginas/SIPC-Tasa-de-Homicidios-Basada-en-reporte-de-homicidios-de-la-Policia-Nacional.aspx</t>
-  </si>
-  <si>
     <t>Casos de violencia física notificados en el dpto. del Cauca</t>
   </si>
   <si>
@@ -1114,24 +1090,12 @@
     <t xml:space="preserve">https://www.sispro.gov.co/observatorios/onviolenciasgenero/Paginas/home.aspx </t>
   </si>
   <si>
-    <t>https://observatoriofeminicidioscolombia.org/reportes</t>
-  </si>
-  <si>
-    <t>H02</t>
-  </si>
-  <si>
-    <t>FEM02</t>
-  </si>
-  <si>
     <t>VS02</t>
   </si>
   <si>
     <t>VF01</t>
   </si>
   <si>
-    <t>L​a Tasa de Homicidios, es indicador básico en materia de política criminal y mide la cantidad de personas por cada 100 mil habitantes que perdieron la vida a causa de un homicidio.El presente indicador es calculado por el observatorio de política criminal tomando 2 fuentes: Reportes de homicidios suministrados por  la Policia Nacional - DIJIN y la cantidad de población reportada por el DANE.El reporte está jerarquizado a nivel departamental y municipal.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desempleo juvenil </t>
   </si>
   <si>
@@ -1219,12 +1183,6 @@
     <t>Número homicidios por circunstancia de feminicidio, según escenario del hecho en el depto. del Cauca.</t>
   </si>
   <si>
-    <t>Republicanas Populares </t>
-  </si>
-  <si>
-    <t>Mujeres, etnia</t>
-  </si>
-  <si>
     <t>​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​​Observatorio Nacional de Violencias de Género</t>
   </si>
   <si>
@@ -1573,9 +1531,6 @@
     <t>(Numero total de nacidos vivos de madres    residentes en el Cauca en un año / Poblacion total residente en el Cauca a mitad de ese año)×1000</t>
   </si>
   <si>
-    <t>Numero total de casos de feminicidio en mujeres del Cauca en el año t</t>
-  </si>
-  <si>
     <t>Numero total de casos de violencia fısica notificados en el Cauca en el año t</t>
   </si>
   <si>
@@ -1640,9 +1595,6 @@
   </si>
   <si>
     <t>Encuesta Nacional de Calidad de Vida para población campesina 2024</t>
-  </si>
-  <si>
-    <t>Tasa de Homicidios (Basada en reporte de homicidios de la Policía Nacional)</t>
   </si>
   <si>
     <t>https://estadisticaselectorales.registraduria.gov.co/unit?str_opc=Elecciones%20Territoriales%20Alcald%C3%ADa&amp;idFilter=3&amp;filter=TERRITORIALES&amp;t=TERRITORIALES&amp;y1=2023&amp;i1=41&amp;y2=false&amp;i2=0</t>
@@ -1753,9 +1705,6 @@
     <t xml:space="preserve">El indicador permitirá medir la participación de las mujeres en cargos de elección popular y poder político en las Juntas Administradoras Locales (JAL) según sexo. A nivel temporal permitirá analizar la magnitud de la participación de la mujer en escenarios de poder político, en términos de permitir un acercamiento a la evolución de la participación política de la mujer en el departamento del Cauca.
 Este indicador se encuentra alineado con la batería de indicadores del Observatorio Colombiano de las Mujeres (indicador trazador).  
 </t>
-  </si>
-  <si>
-    <t>(Numero total de homicidios en el Cauca en el año, segun sexo/Poblacion total del Cauca del mismo sexo en el mismo año)×100.000</t>
   </si>
   <si>
     <t>ART-01</t>
@@ -1962,28 +1911,6 @@
         <scheme val="major"/>
       </rPr>
       <t xml:space="preserve"> descargada del portal de datos del  Centro Nacional de Memoria Histórica y Observatorio de Memoria y Conflicto</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Violencia física</t>
     </r>
   </si>
   <si>
@@ -2234,6 +2161,28 @@
   </si>
   <si>
     <t>XLS, CSV</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Violencia física</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2702,7 +2651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2903,9 +2852,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2959,6 +2905,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2972,9 +2921,6 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3253,76 +3199,76 @@
       <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:20" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="80" t="s">
+      <c r="P2" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>93</v>
@@ -3331,22 +3277,22 @@
         <v>274</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="N3" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>28</v>
@@ -3357,46 +3303,46 @@
     </row>
     <row r="4" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>483</v>
+        <v>468</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="L4" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="N4" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O4" s="31" t="s">
         <v>28</v>
@@ -3406,19 +3352,19 @@
     </row>
     <row r="5" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>539</v>
+        <v>522</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>21</v>
@@ -3427,25 +3373,25 @@
         <v>93</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>535</v>
+        <v>518</v>
       </c>
       <c r="L5" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>537</v>
+        <v>520</v>
       </c>
       <c r="O5" s="31" t="s">
         <v>28</v>
@@ -3455,46 +3401,46 @@
     </row>
     <row r="6" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="L6" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>28</v>
@@ -3504,19 +3450,19 @@
     </row>
     <row r="7" spans="1:20" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -3525,25 +3471,25 @@
         <v>93</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
       <c r="L7" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="N7" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O7" s="31" t="s">
         <v>28</v>
@@ -3553,19 +3499,19 @@
     </row>
     <row r="8" spans="1:20" ht="409.2" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>412</v>
-      </c>
       <c r="D8" s="14" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>21</v>
@@ -3574,32 +3520,32 @@
         <v>93</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="L8" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O8" s="31"/>
       <c r="P8" s="12" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="Q8" s="14" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3632,8 +3578,8 @@
   </sheetPr>
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3673,55 +3619,55 @@
       <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="82" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="81" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="81" t="s">
+      <c r="P2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="Q2" s="80" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3763,10 +3709,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="63" t="s">
-        <v>551</v>
-      </c>
-      <c r="N3" s="87" t="s">
-        <v>512</v>
+        <v>533</v>
+      </c>
+      <c r="N3" s="86" t="s">
+        <v>496</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>130</v>
@@ -3814,10 +3760,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>552</v>
-      </c>
-      <c r="N4" s="87" t="s">
-        <v>512</v>
+        <v>534</v>
+      </c>
+      <c r="N4" s="86" t="s">
+        <v>496</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>130</v>
@@ -3841,7 +3787,7 @@
         <v>204</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>205</v>
@@ -3867,8 +3813,8 @@
       <c r="M5" s="63" t="s">
         <v>208</v>
       </c>
-      <c r="N5" s="87" t="s">
-        <v>512</v>
+      <c r="N5" s="86" t="s">
+        <v>496</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
@@ -3892,7 +3838,7 @@
         <v>211</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>212</v>
@@ -3915,11 +3861,11 @@
       <c r="L6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="88" t="s">
-        <v>553</v>
-      </c>
-      <c r="N6" s="87" t="s">
-        <v>513</v>
+      <c r="M6" s="87" t="s">
+        <v>535</v>
+      </c>
+      <c r="N6" s="86" t="s">
+        <v>497</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
@@ -3931,7 +3877,7 @@
     </row>
     <row r="7" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>188</v>
@@ -4015,11 +3961,11 @@
       <c r="L8" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="89" t="s">
+      <c r="M8" s="88" t="s">
         <v>236</v>
       </c>
-      <c r="N8" s="90" t="s">
-        <v>514</v>
+      <c r="N8" s="89" t="s">
+        <v>498</v>
       </c>
       <c r="O8" s="27" t="s">
         <v>130</v>
@@ -4041,19 +3987,19 @@
     </row>
     <row r="9" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="B9" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="90" t="s">
         <v>270</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>269</v>
@@ -4065,49 +4011,49 @@
         <v>94</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="L9" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B10" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="91" t="s">
-        <v>311</v>
+      <c r="C10" s="90" t="s">
+        <v>303</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>193</v>
@@ -4116,22 +4062,22 @@
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="L10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>130</v>
@@ -4141,203 +4087,203 @@
     </row>
     <row r="11" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="B11" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="91" t="s">
-        <v>369</v>
-      </c>
-      <c r="D11" s="91" t="s">
-        <v>440</v>
+      <c r="C11" s="90" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" s="90" t="s">
+        <v>426</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="L11" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="N11" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O11" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="29" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="B12" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="91" t="s">
-        <v>372</v>
-      </c>
-      <c r="D12" s="91" t="s">
-        <v>373</v>
+      <c r="C12" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="D12" s="90" t="s">
+        <v>359</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="L12" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="N12" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O12" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="29" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="D13" s="91" t="s">
-        <v>433</v>
-      </c>
-      <c r="E13" s="91" t="s">
-        <v>443</v>
-      </c>
-      <c r="F13" s="91" t="s">
-        <v>434</v>
-      </c>
-      <c r="G13" s="91" t="s">
+      <c r="D13" s="90" t="s">
+        <v>419</v>
+      </c>
+      <c r="E13" s="90" t="s">
+        <v>429</v>
+      </c>
+      <c r="F13" s="90" t="s">
+        <v>420</v>
+      </c>
+      <c r="G13" s="90" t="s">
         <v>193</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="L13" s="91" t="s">
+        <v>418</v>
+      </c>
+      <c r="L13" s="90" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="N13" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O13" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P13" s="91"/>
-      <c r="Q13" s="91"/>
+      <c r="P13" s="90"/>
+      <c r="Q13" s="90"/>
     </row>
     <row r="14" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B14" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="91" t="s">
-        <v>444</v>
-      </c>
-      <c r="E14" s="91" t="s">
-        <v>429</v>
-      </c>
-      <c r="F14" s="91" t="s">
+      <c r="D14" s="90" t="s">
         <v>430</v>
       </c>
-      <c r="G14" s="91" t="s">
+      <c r="E14" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="F14" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="G14" s="90" t="s">
         <v>193</v>
       </c>
-      <c r="H14" s="91" t="s">
+      <c r="H14" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="91" t="s">
-        <v>466</v>
+      <c r="I14" s="90" t="s">
+        <v>452</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="L14" s="91" t="s">
+        <v>418</v>
+      </c>
+      <c r="L14" s="90" t="s">
         <v>27</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="N14" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O14" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4366,10 +4312,10 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4409,55 +4355,55 @@
       <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="1:30" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="81" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="80" t="s">
+      <c r="P2" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="Q2" s="79" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="2"/>
@@ -4485,10 +4431,10 @@
         <v>61</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>62</v>
@@ -4512,10 +4458,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>68</v>
@@ -4529,7 +4475,7 @@
     </row>
     <row r="4" spans="1:30" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>60</v>
@@ -4538,7 +4484,7 @@
         <v>61</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>276</v>
@@ -4553,13 +4499,13 @@
         <v>94</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>27</v>
@@ -4568,14 +4514,14 @@
         <v>280</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="14" t="s">
-        <v>546</v>
+        <v>529</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="211.2" x14ac:dyDescent="0.25">
@@ -4589,10 +4535,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>73</v>
@@ -4616,10 +4562,10 @@
         <v>27</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="N5" s="18" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>68</v>
@@ -4643,7 +4589,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>21</v>
@@ -4667,10 +4613,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>68</v>
@@ -4691,10 +4637,10 @@
         <v>83</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>268</v>
@@ -4718,10 +4664,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O7" s="27" t="s">
         <v>86</v>
@@ -4736,176 +4682,171 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="237.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
-        <v>320</v>
-      </c>
-      <c r="B8" s="70" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>83</v>
+      <c r="C8" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>127</v>
+        <v>340</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="H8" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="29" t="s">
-        <v>531</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>495</v>
+      <c r="J8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="L8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="N8" s="48" t="s">
-        <v>512</v>
+      <c r="M8" s="20" t="s">
+        <v>528</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>307</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>247</v>
-      </c>
-      <c r="P8" s="71" t="s">
-        <v>324</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="P8" s="14"/>
       <c r="Q8" s="29"/>
-      <c r="AD8" s="3"/>
-    </row>
-    <row r="9" spans="1:30" ht="132" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="s">
-        <v>90</v>
+    </row>
+    <row r="9" spans="1:30" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>91</v>
+        <v>540</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>353</v>
+        <v>298</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>93</v>
+        <v>435</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>127</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>67</v>
+        <v>458</v>
+      </c>
+      <c r="J9" s="71" t="s">
+        <v>300</v>
+      </c>
+      <c r="K9" s="71" t="s">
+        <v>342</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="20" t="s">
-        <v>545</v>
+      <c r="M9" s="72" t="s">
+        <v>301</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>315</v>
+        <v>496</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="29"/>
-    </row>
-    <row r="10" spans="1:30" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="69" t="s">
-        <v>321</v>
+        <v>130</v>
+      </c>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:30" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>486</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>91</v>
+        <v>308</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>298</v>
+        <v>436</v>
       </c>
       <c r="E10" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="F10" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="29" t="s">
         <v>93</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>472</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="K10" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="J10" s="71" t="s">
         <v>300</v>
+      </c>
+      <c r="K10" s="71" t="s">
+        <v>342</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="N10" s="29" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="71" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q10" s="29"/>
-    </row>
-    <row r="11" spans="1:30" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:30" ht="66" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="72" t="s">
-        <v>547</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>449</v>
+      <c r="C11" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>275</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>127</v>
@@ -4914,120 +4855,22 @@
         <v>94</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>473</v>
-      </c>
-      <c r="J11" s="71" t="s">
-        <v>308</v>
-      </c>
-      <c r="K11" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="73" t="s">
-        <v>309</v>
-      </c>
-      <c r="N11" s="29" t="s">
-        <v>512</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
       <c r="O11" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="P11" s="16"/>
+        <v>273</v>
+      </c>
+      <c r="P11" s="73"/>
       <c r="Q11" s="16"/>
-    </row>
-    <row r="12" spans="1:30" ht="118.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>450</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>474</v>
-      </c>
-      <c r="J12" s="71" t="s">
-        <v>308</v>
-      </c>
-      <c r="K12" s="71" t="s">
-        <v>356</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>512</v>
-      </c>
-      <c r="O12" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-    </row>
-    <row r="13" spans="1:30" ht="66" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>357</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>358</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="J13" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5035,19 +4878,17 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M8" r:id="rId1" xr:uid="{8E281984-9540-4FB0-B503-73B6103B303B}"/>
-    <hyperlink ref="M11" r:id="rId2" xr:uid="{797ABC50-2A20-4AAF-9B90-2592052B5F18}"/>
-    <hyperlink ref="M4" r:id="rId3" xr:uid="{07A6CABB-F701-496C-8CB0-2E7AD48C8E0D}"/>
-    <hyperlink ref="M12" r:id="rId4" xr:uid="{1C03CBF7-CD9E-49B3-906D-D76865D2C898}"/>
-    <hyperlink ref="M10" r:id="rId5" xr:uid="{7B5F8912-C261-4A9C-BBCF-0C83BCE367D6}"/>
-    <hyperlink ref="M3" r:id="rId6" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{B59D45E6-480A-4ED5-9E19-023515EF3F58}"/>
-    <hyperlink ref="M5" r:id="rId7" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{729BE810-B166-4B8D-9966-0F9DDF8CA789}"/>
-    <hyperlink ref="M6" r:id="rId8" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{D8082A5C-A96F-4ADB-B9D9-5DFCF268FE98}"/>
-    <hyperlink ref="M7" r:id="rId9" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{2F23AC26-6244-4829-B396-B8ADE3106207}"/>
-    <hyperlink ref="M9" r:id="rId10" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{26F98D13-D80F-4F6C-8D50-30C433C8FD32}"/>
+    <hyperlink ref="M9" r:id="rId1" xr:uid="{797ABC50-2A20-4AAF-9B90-2592052B5F18}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{07A6CABB-F701-496C-8CB0-2E7AD48C8E0D}"/>
+    <hyperlink ref="M10" r:id="rId3" xr:uid="{1C03CBF7-CD9E-49B3-906D-D76865D2C898}"/>
+    <hyperlink ref="M3" r:id="rId4" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{B59D45E6-480A-4ED5-9E19-023515EF3F58}"/>
+    <hyperlink ref="M5" r:id="rId5" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{729BE810-B166-4B8D-9966-0F9DDF8CA789}"/>
+    <hyperlink ref="M6" r:id="rId6" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{D8082A5C-A96F-4ADB-B9D9-5DFCF268FE98}"/>
+    <hyperlink ref="M7" r:id="rId7" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{2F23AC26-6244-4829-B396-B8ADE3106207}"/>
+    <hyperlink ref="M8" r:id="rId8" display="https://www.medicinalegal.gov.co/cifras-estadisticas/boletines-estadisticos-nna " xr:uid="{26F98D13-D80F-4F6C-8D50-30C433C8FD32}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -5099,55 +4940,55 @@
       <c r="Q1" s="97"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="81" t="s">
+      <c r="P2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="Q2" s="80" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5192,7 +5033,7 @@
         <v>140</v>
       </c>
       <c r="N3" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>130</v>
@@ -5243,7 +5084,7 @@
         <v>146</v>
       </c>
       <c r="N4" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>130</v>
@@ -5294,7 +5135,7 @@
         <v>154</v>
       </c>
       <c r="N5" s="62" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
@@ -5345,7 +5186,7 @@
         <v>154</v>
       </c>
       <c r="N6" s="62" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
@@ -5393,10 +5234,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
       <c r="N7" s="60" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="O7" s="19" t="s">
         <v>130</v>
@@ -5447,7 +5288,7 @@
         <v>169</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="O8" s="19" t="s">
         <v>130</v>
@@ -5459,7 +5300,7 @@
     </row>
     <row r="9" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>132</v>
@@ -5495,10 +5336,10 @@
         <v>27</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="N9" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O9" s="19" t="s">
         <v>130</v>
@@ -5516,13 +5357,13 @@
         <v>132</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>21</v>
@@ -5540,16 +5381,16 @@
         <v>138</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="N10" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O10" s="19" t="s">
         <v>130</v>
@@ -5627,55 +5468,55 @@
       <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="81" t="s">
+      <c r="M2" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>341</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>329</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="81" t="s">
+      <c r="P2" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="81" t="s">
+      <c r="Q2" s="80" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5693,7 +5534,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>100</v>
@@ -5762,10 +5603,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>105</v>
@@ -5813,16 +5654,16 @@
         <v>27</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>119</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="Q5" s="30"/>
     </row>
@@ -5840,7 +5681,7 @@
         <v>122</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>21</v>
@@ -5852,7 +5693,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="J6" s="29" t="s">
         <v>112</v>
@@ -5864,10 +5705,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>119</v>
@@ -5879,7 +5720,7 @@
     </row>
     <row r="7" spans="1:17" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>97</v>
@@ -5888,10 +5729,10 @@
         <v>108</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -5903,7 +5744,7 @@
         <v>42</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="J7" s="29" t="s">
         <v>112</v>
@@ -5915,16 +5756,16 @@
         <v>27</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="O7" s="29" t="s">
         <v>119</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="Q7" s="31"/>
     </row>
@@ -5942,7 +5783,7 @@
         <v>125</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>126</v>
@@ -5973,19 +5814,19 @@
     </row>
     <row r="9" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>486</v>
+        <v>471</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>487</v>
+        <v>472</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>488</v>
+        <v>473</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>21</v>
@@ -5997,22 +5838,22 @@
         <v>42</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O9" s="57" t="s">
         <v>130</v>
@@ -6047,7 +5888,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -6088,55 +5929,55 @@
       <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="82" t="s">
+      <c r="M2" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="83" t="s">
+      <c r="P2" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="83" t="s">
+      <c r="Q2" s="82" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6154,7 +5995,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>21</v>
@@ -6178,10 +6019,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="N3" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>28</v>
@@ -6205,7 +6046,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>267</v>
@@ -6232,7 +6073,7 @@
         <v>32</v>
       </c>
       <c r="N4" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>28</v>
@@ -6285,7 +6126,7 @@
         <v>32</v>
       </c>
       <c r="N5" s="60" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>28</v>
@@ -6297,7 +6138,7 @@
     </row>
     <row r="6" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>18</v>
@@ -6333,10 +6174,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="N6" s="100" t="s">
-        <v>556</v>
+        <v>331</v>
+      </c>
+      <c r="N6" s="91" t="s">
+        <v>538</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>28</v>
@@ -6348,7 +6189,7 @@
     </row>
     <row r="7" spans="1:17" ht="343.2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>45</v>
@@ -6384,10 +6225,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="N7" s="100" t="s">
-        <v>556</v>
+        <v>331</v>
+      </c>
+      <c r="N7" s="91" t="s">
+        <v>538</v>
       </c>
       <c r="O7" s="25" t="s">
         <v>28</v>
@@ -6399,7 +6240,7 @@
     </row>
     <row r="8" spans="1:17" ht="369.6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>45</v>
@@ -6435,10 +6276,10 @@
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>555</v>
+        <v>537</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="O8" s="29" t="s">
         <v>28</v>
@@ -6456,25 +6297,25 @@
         <v>18</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="H9" s="31" t="s">
         <v>274</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>25</v>
@@ -6486,32 +6327,32 @@
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>21</v>
@@ -6523,22 +6364,22 @@
         <v>274</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="L10" s="34" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O10" s="34" t="s">
         <v>28</v>
@@ -6554,43 +6395,43 @@
         <v>18</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="H11" s="31" t="s">
         <v>274</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="L11" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="N11" s="31" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
@@ -7024,55 +6865,55 @@
       <c r="Q1" s="95"/>
     </row>
     <row r="2" spans="1:17" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="M2" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="85" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="86" t="s">
+      <c r="N2" s="84" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="83" t="s">
+      <c r="P2" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="83" t="s">
+      <c r="Q2" s="82" t="s">
         <v>16</v>
       </c>
     </row>
@@ -7081,7 +6922,7 @@
         <v>238</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>239</v>
@@ -7127,10 +6968,10 @@
     </row>
     <row r="4" spans="1:17" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>250</v>
@@ -7179,7 +7020,7 @@
         <v>249</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>250</v>
@@ -7228,7 +7069,7 @@
         <v>259</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>278</v>
@@ -7249,13 +7090,13 @@
         <v>94</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="L6" s="46" t="s">
         <v>27</v>
@@ -7264,22 +7105,22 @@
         <v>280</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O6" s="43" t="s">
         <v>130</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>281</v>
@@ -7300,13 +7141,13 @@
         <v>94</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="J7" s="49" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="L7" s="46" t="s">
         <v>27</v>
@@ -7315,22 +7156,22 @@
         <v>280</v>
       </c>
       <c r="N7" s="48" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O7" s="43" t="s">
         <v>130</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>282</v>
@@ -7351,7 +7192,7 @@
         <v>94</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>283</v>
@@ -7364,7 +7205,7 @@
         <v>284</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O8" s="50" t="s">
         <v>287</v>
@@ -7374,10 +7215,10 @@
     </row>
     <row r="9" spans="1:17" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>285</v>
@@ -7398,7 +7239,7 @@
         <v>94</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>283</v>
@@ -7411,7 +7252,7 @@
         <v>286</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="O9" s="50" t="s">
         <v>287</v>
@@ -7421,22 +7262,22 @@
     </row>
     <row r="10" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="G10" s="46" t="s">
         <v>193</v>
@@ -7445,22 +7286,22 @@
         <v>94</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="L10" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>247</v>
@@ -7538,73 +7379,73 @@
       <c r="Q1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="I2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="79" t="s">
+      <c r="J2" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="79" t="s">
+      <c r="K2" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="78" t="s">
+      <c r="L2" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="78" t="s">
+      <c r="M2" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="79" t="s">
-        <v>312</v>
-      </c>
-      <c r="O2" s="78" t="s">
+      <c r="N2" s="78" t="s">
+        <v>304</v>
+      </c>
+      <c r="O2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="79" t="s">
+      <c r="P2" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="77" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>21</v>
@@ -7613,77 +7454,77 @@
         <v>193</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>534</v>
+        <v>517</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>510</v>
+        <v>494</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>

</xml_diff>

<commit_message>
Se realizo el ajuste de la bateria en base a las sugerencias del marco conceptual
</commit_message>
<xml_diff>
--- a/data/Cauca_Bateria de indicadores V1 .xlsx
+++ b/data/Cauca_Bateria de indicadores V1 .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\observatorio-mujer-cauca\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1DD80C-0861-457F-85C3-DCB7CE1B8FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE36F858-0A89-4A70-9073-06FFFBB0378E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sociodemografico" sheetId="8" r:id="rId1"/>
@@ -629,44 +629,6 @@
   </si>
   <si>
     <t>POrcentaje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se realiza a través de la auto clasificación de las personas en los niveles educativos establecidos en el formulario de la GEIH y el título de mayor nivel educativo alcanzado. Se deben sumar las variables de nivel y título educativo creando la variable de la Clasificación Internacional Normalizada de la Educación - niveles de educación adaptada para Colombia. Cine-N 2011 A.C. con los siguientes niveles:
-Ninguno
-CINE 1 - educación básica primaria
-CINE 2 - educación básica secundaria
-CINE 3 - educación Media
-CINE 5 - educación técnica profesional y tecnológica
-CINE 6 - educación superior
-CINE 7-8 - postgrado
-No determinado
-Cálculo en R:
-Para realizar los cálculos de indicadores de nivel educativo se utilizan las variables P6210, P6210s1 y P6220
-Se deben sumar los valores de las variables P6210 y P6210S1, construyendo la variable Educ.
-Luego se utiliza la siguiente función
-When Calculated Educ Between '100' and '304'                               Then 0
-When Calculated Educ Between '305' and '408'                               Then 1
-When Calculated Educ Between '409' and '513' and p6220 not &gt;1  Then 2
-When Calculated Educ in ('511')and p6220 in(1)                               Then 2 
-When Calculated Educ &gt;='511' and P6220 in(2)                                Then 3
-When Calculated Educ &gt;='601' and P6220 in(3)                                Then 5
-When Calculated Educ &gt;='604' and P6220 in(4)                                Then 6
-When Calculated Educ &gt;='605' and P6220 in(5)                                Then 7
-When Calculated Educ &gt;='500' and P6220 in(9)                                Then 99
-When Calculated Educ in('900') or Calculated Educ in('999') 
-or p6220=9                                                                                         Then 99
-Else 98 End As CINE11 Label='CINE 2011',
-Finalmente se utiliza el siguiente formato con los valores obtenidos en la función condicional anterior.
-0='Ninguno'
-1='CINE 1 - educación básica primaria'
-2='CINE 2 - educación básica secundaria'
-3='CINE 3 - educación Media'
-5='CINE 5 - educación técnica profesional y tecnológica'
-6='CINE 6 - educación superior'
-7='CINE 7-8 - postgrado'
-99='No informa'
-98='No determinado';
-</t>
   </si>
   <si>
     <t xml:space="preserve">Los resultados del indicador muestran la distribución de la población de 25 a 64 años (dividido en los grupos: 25-34, 35-44, 45-54 y 55-64) de acuerdo con el nivel educativo alcanzado (sin primaria, primaria, secundaria, media superior y superior).
@@ -2183,6 +2145,10 @@
       </rPr>
       <t>Violencia física</t>
     </r>
+  </si>
+  <si>
+    <t>(Proporción de personas entre 25 y 64 años según máximo nivel educativo alcanzado y sexo) = (Número total de personas entre 25 y 64 años con determinado nivel educativo y sexo / Total de personas entre 25 y 64 años del mismo sexo) × 100 
+Para realizar los cálculos de indicadores de nivel educativo se utilizan las variables P6210, P6210s1 y P6220</t>
   </si>
 </sst>
 </file>
@@ -3239,7 +3205,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -3253,46 +3219,46 @@
     </row>
     <row r="3" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>485</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J3" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N3" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O3" s="31" t="s">
         <v>28</v>
@@ -3303,46 +3269,46 @@
     </row>
     <row r="4" spans="1:20" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>386</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>482</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="F4" s="29" t="s">
         <v>388</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>389</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>93</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L4" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N4" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O4" s="31" t="s">
         <v>28</v>
@@ -3352,19 +3318,19 @@
     </row>
     <row r="5" spans="1:20" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>390</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>521</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>522</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>391</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>21</v>
@@ -3373,25 +3339,25 @@
         <v>93</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L5" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="N5" s="48" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O5" s="31" t="s">
         <v>28</v>
@@ -3401,46 +3367,46 @@
     </row>
     <row r="6" spans="1:20" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>501</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>392</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>500</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>499</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>501</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="H6" s="31" t="s">
+        <v>364</v>
+      </c>
+      <c r="I6" s="29" t="s">
         <v>502</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>365</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>503</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L6" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O6" s="31" t="s">
         <v>28</v>
@@ -3450,19 +3416,19 @@
     </row>
     <row r="7" spans="1:20" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>400</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>401</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -3471,25 +3437,25 @@
         <v>93</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L7" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N7" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O7" s="31" t="s">
         <v>28</v>
@@ -3499,19 +3465,19 @@
     </row>
     <row r="8" spans="1:20" ht="409.2" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>404</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>21</v>
@@ -3520,32 +3486,32 @@
         <v>93</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L8" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O8" s="31"/>
       <c r="P8" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q8" s="14" t="s">
         <v>531</v>
-      </c>
-      <c r="Q8" s="14" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3659,7 +3625,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -3673,305 +3639,305 @@
     </row>
     <row r="3" spans="1:27" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>196</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>197</v>
       </c>
       <c r="L3" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="63" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="N3" s="86" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q3" s="21"/>
     </row>
     <row r="4" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="E4" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="F4" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>202</v>
-      </c>
       <c r="J4" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>196</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>197</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="N4" s="86" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q4" s="21"/>
     </row>
     <row r="5" spans="1:27" ht="343.2" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M5" s="63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N5" s="86" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q5" s="21"/>
     </row>
     <row r="6" spans="1:27" ht="250.8" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="J6" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" s="18" t="s">
         <v>215</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>216</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="87" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N6" s="86" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="F7" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>222</v>
-      </c>
       <c r="G7" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>42</v>
       </c>
       <c r="I7" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="K7" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="L7" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="M7" s="18" t="s">
         <v>226</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>227</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="P7" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>229</v>
       </c>
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C8" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="E8" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>233</v>
-      </c>
       <c r="G8" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H8" s="27" t="s">
         <v>42</v>
       </c>
       <c r="I8" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="K8" s="26" t="s">
         <v>234</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>196</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>235</v>
       </c>
       <c r="L8" s="27" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="88" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N8" s="89" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="O8" s="27" t="s">
         <v>130</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q8" s="21"/>
       <c r="R8" s="3"/>
@@ -3987,97 +3953,97 @@
     </row>
     <row r="9" spans="1:27" ht="132" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" s="29" t="s">
         <v>421</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>422</v>
-      </c>
       <c r="F9" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>94</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L9" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>425</v>
-      </c>
       <c r="F10" s="29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>130</v>
@@ -4087,148 +4053,148 @@
     </row>
     <row r="11" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B11" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" s="90" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" s="90" t="s">
+        <v>425</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="D11" s="90" t="s">
-        <v>426</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>356</v>
-      </c>
       <c r="G11" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L11" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N11" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O11" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" s="90" t="s">
+        <v>357</v>
+      </c>
+      <c r="D12" s="90" t="s">
         <v>358</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="E12" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>355</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>359</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>356</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>360</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L12" s="29" t="s">
         <v>27</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="N12" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O12" s="29" t="s">
         <v>130</v>
       </c>
       <c r="P12" s="16"/>
       <c r="Q12" s="29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B13" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="90" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="90" t="s">
-        <v>189</v>
-      </c>
       <c r="D13" s="90" t="s">
+        <v>418</v>
+      </c>
+      <c r="E13" s="90" t="s">
+        <v>428</v>
+      </c>
+      <c r="F13" s="90" t="s">
         <v>419</v>
       </c>
-      <c r="E13" s="90" t="s">
-        <v>429</v>
-      </c>
-      <c r="F13" s="90" t="s">
-        <v>420</v>
-      </c>
       <c r="G13" s="90" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J13" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="K13" s="14" t="s">
         <v>417</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>418</v>
       </c>
       <c r="L13" s="90" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N13" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O13" s="29" t="s">
         <v>130</v>
@@ -4238,46 +4204,46 @@
     </row>
     <row r="14" spans="1:27" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
+        <v>413</v>
+      </c>
+      <c r="B14" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="90" t="s">
+        <v>429</v>
+      </c>
+      <c r="E14" s="90" t="s">
         <v>414</v>
       </c>
-      <c r="B14" s="70" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="90" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="90" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="90" t="s">
+      <c r="F14" s="90" t="s">
         <v>415</v>
       </c>
-      <c r="F14" s="90" t="s">
-        <v>416</v>
-      </c>
       <c r="G14" s="90" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H14" s="90" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="90" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J14" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>417</v>
-      </c>
-      <c r="K14" s="14" t="s">
-        <v>418</v>
       </c>
       <c r="L14" s="90" t="s">
         <v>27</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N14" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O14" s="29" t="s">
         <v>130</v>
@@ -4314,7 +4280,7 @@
   </sheetPr>
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -4392,10 +4358,10 @@
         <v>12</v>
       </c>
       <c r="M2" s="81" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -4431,10 +4397,10 @@
         <v>61</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>62</v>
@@ -4458,10 +4424,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>68</v>
@@ -4475,7 +4441,7 @@
     </row>
     <row r="4" spans="1:30" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>60</v>
@@ -4484,13 +4450,13 @@
         <v>61</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>276</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>277</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>127</v>
@@ -4499,29 +4465,29 @@
         <v>94</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J4" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>433</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>434</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O4" s="14" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="211.2" x14ac:dyDescent="0.25">
@@ -4535,10 +4501,10 @@
         <v>72</v>
       </c>
       <c r="D5" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>335</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>336</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>73</v>
@@ -4562,10 +4528,10 @@
         <v>27</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N5" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O5" s="18" t="s">
         <v>68</v>
@@ -4589,7 +4555,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>21</v>
@@ -4613,10 +4579,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>68</v>
@@ -4637,13 +4603,13 @@
         <v>83</v>
       </c>
       <c r="D7" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>338</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>339</v>
-      </c>
       <c r="F7" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>63</v>
@@ -4664,10 +4630,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O7" s="27" t="s">
         <v>86</v>
@@ -4693,10 +4659,10 @@
         <v>91</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>92</v>
@@ -4720,10 +4686,10 @@
         <v>27</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N8" s="29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O8" s="29" t="s">
         <v>86</v>
@@ -4733,22 +4699,22 @@
     </row>
     <row r="9" spans="1:30" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>127</v>
@@ -4757,22 +4723,22 @@
         <v>94</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J9" s="71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L9" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="72" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N9" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O9" s="29" t="s">
         <v>130</v>
@@ -4782,22 +4748,22 @@
     </row>
     <row r="10" spans="1:30" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>436</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>309</v>
-      </c>
       <c r="F10" s="29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>93</v>
@@ -4806,22 +4772,22 @@
         <v>94</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J10" s="71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L10" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N10" s="29" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O10" s="29" t="s">
         <v>130</v>
@@ -4831,22 +4797,22 @@
     </row>
     <row r="11" spans="1:30" ht="66" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>344</v>
-      </c>
       <c r="E11" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>127</v>
@@ -4858,7 +4824,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>67</v>
@@ -4867,7 +4833,7 @@
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P11" s="73"/>
       <c r="Q11" s="16"/>
@@ -4900,8 +4866,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4980,7 +4946,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -5033,7 +4999,7 @@
         <v>140</v>
       </c>
       <c r="N3" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>130</v>
@@ -5084,7 +5050,7 @@
         <v>146</v>
       </c>
       <c r="N4" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>130</v>
@@ -5135,7 +5101,7 @@
         <v>154</v>
       </c>
       <c r="N5" s="62" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>130</v>
@@ -5186,7 +5152,7 @@
         <v>154</v>
       </c>
       <c r="N6" s="62" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>130</v>
@@ -5234,10 +5200,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N7" s="60" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O7" s="19" t="s">
         <v>130</v>
@@ -5247,7 +5213,7 @@
       </c>
       <c r="Q7" s="21"/>
     </row>
-    <row r="8" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>171</v>
       </c>
@@ -5273,7 +5239,7 @@
         <v>176</v>
       </c>
       <c r="I8" s="59" t="s">
-        <v>177</v>
+        <v>540</v>
       </c>
       <c r="J8" s="19" t="s">
         <v>25</v>
@@ -5288,34 +5254,34 @@
         <v>169</v>
       </c>
       <c r="N8" s="60" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="O8" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P8" s="59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q8" s="21"/>
     </row>
     <row r="9" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="F9" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>183</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>93</v>
@@ -5324,46 +5290,46 @@
         <v>42</v>
       </c>
       <c r="I9" s="59" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L9" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N9" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O9" s="19" t="s">
         <v>130</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:17" ht="66" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>132</v>
       </c>
       <c r="C10" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>377</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>379</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>378</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>21</v>
@@ -5381,16 +5347,16 @@
         <v>138</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N10" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O10" s="19" t="s">
         <v>130</v>
@@ -5508,7 +5474,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -5534,7 +5500,7 @@
         <v>99</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>100</v>
@@ -5603,10 +5569,10 @@
         <v>27</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>105</v>
@@ -5654,16 +5620,16 @@
         <v>27</v>
       </c>
       <c r="M5" s="23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>119</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="Q5" s="30"/>
     </row>
@@ -5681,7 +5647,7 @@
         <v>122</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>21</v>
@@ -5693,7 +5659,7 @@
         <v>42</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J6" s="29" t="s">
         <v>112</v>
@@ -5705,10 +5671,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>119</v>
@@ -5720,7 +5686,7 @@
     </row>
     <row r="7" spans="1:17" ht="224.4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>97</v>
@@ -5729,10 +5695,10 @@
         <v>108</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>21</v>
@@ -5744,7 +5710,7 @@
         <v>42</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J7" s="29" t="s">
         <v>112</v>
@@ -5756,16 +5722,16 @@
         <v>27</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O7" s="29" t="s">
         <v>119</v>
       </c>
       <c r="P7" s="29" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q7" s="31"/>
     </row>
@@ -5783,7 +5749,7 @@
         <v>125</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F8" s="53" t="s">
         <v>126</v>
@@ -5814,19 +5780,19 @@
     </row>
     <row r="9" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>472</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>473</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>474</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>21</v>
@@ -5838,22 +5804,22 @@
         <v>42</v>
       </c>
       <c r="I9" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="K9" s="14" t="s">
         <v>476</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>477</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O9" s="57" t="s">
         <v>130</v>
@@ -5969,7 +5935,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="81" t="s">
         <v>14</v>
@@ -5995,7 +5961,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>21</v>
@@ -6019,10 +5985,10 @@
         <v>27</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N3" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>28</v>
@@ -6046,10 +6012,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>22</v>
@@ -6073,7 +6039,7 @@
         <v>32</v>
       </c>
       <c r="N4" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O4" s="19" t="s">
         <v>28</v>
@@ -6126,7 +6092,7 @@
         <v>32</v>
       </c>
       <c r="N5" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>28</v>
@@ -6138,7 +6104,7 @@
     </row>
     <row r="6" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>18</v>
@@ -6174,10 +6140,10 @@
         <v>27</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N6" s="91" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>28</v>
@@ -6189,7 +6155,7 @@
     </row>
     <row r="7" spans="1:17" ht="343.2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>45</v>
@@ -6225,10 +6191,10 @@
         <v>27</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N7" s="91" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O7" s="25" t="s">
         <v>28</v>
@@ -6240,7 +6206,7 @@
     </row>
     <row r="8" spans="1:17" ht="369.6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>45</v>
@@ -6276,10 +6242,10 @@
         <v>27</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O8" s="29" t="s">
         <v>28</v>
@@ -6297,25 +6263,25 @@
         <v>18</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="F9" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="F9" s="31" t="s">
+      <c r="G9" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>317</v>
-      </c>
       <c r="H9" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>25</v>
@@ -6327,32 +6293,32 @@
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="N9" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="O9" s="29" t="s">
         <v>318</v>
-      </c>
-      <c r="N9" s="48" t="s">
-        <v>307</v>
-      </c>
-      <c r="O9" s="29" t="s">
-        <v>319</v>
       </c>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>21</v>
@@ -6361,25 +6327,25 @@
         <v>93</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>25</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L10" s="34" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O10" s="34" t="s">
         <v>28</v>
@@ -6395,43 +6361,43 @@
         <v>18</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>372</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>373</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L11" s="31" t="s">
         <v>27</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N11" s="31" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
@@ -6905,7 +6871,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="84" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="85" t="s">
         <v>14</v>
@@ -6919,392 +6885,392 @@
     </row>
     <row r="3" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="D3" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E3" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>242</v>
-      </c>
       <c r="G3" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I3" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>244</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>245</v>
       </c>
       <c r="L3" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N3" s="39"/>
       <c r="O3" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>247</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>248</v>
       </c>
       <c r="Q3" s="18"/>
     </row>
     <row r="4" spans="1:17" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>253</v>
-      </c>
       <c r="G4" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>94</v>
       </c>
       <c r="I4" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="K4" s="18" t="s">
         <v>255</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>256</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N4" s="39"/>
       <c r="O4" s="40" t="s">
         <v>130</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q4" s="41"/>
     </row>
     <row r="5" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>250</v>
-      </c>
       <c r="D5" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="F5" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>262</v>
-      </c>
       <c r="G5" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>94</v>
       </c>
       <c r="I5" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="J5" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="K5" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="M5" s="42" t="s">
         <v>264</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="M5" s="42" t="s">
-        <v>265</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="43" t="s">
         <v>130</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q5" s="44"/>
     </row>
     <row r="6" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>279</v>
-      </c>
       <c r="G6" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>94</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L6" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N6" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O6" s="43" t="s">
         <v>130</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:17" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H7" s="26" t="s">
         <v>94</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J7" s="49" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L7" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N7" s="48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O7" s="43" t="s">
         <v>130</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="1:17" ht="132" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>94</v>
       </c>
       <c r="I8" s="46" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M8" s="47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N8" s="48" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="O8" s="50" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P8" s="16"/>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>94</v>
       </c>
       <c r="I9" s="46" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M9" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="N9" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="O9" s="50" t="s">
         <v>286</v>
-      </c>
-      <c r="N9" s="48" t="s">
-        <v>305</v>
-      </c>
-      <c r="O9" s="50" t="s">
-        <v>287</v>
       </c>
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:17" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>351</v>
-      </c>
       <c r="G10" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>94</v>
       </c>
       <c r="I10" s="46" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J10" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="K10" s="14" t="s">
         <v>352</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>353</v>
       </c>
       <c r="L10" s="46" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
@@ -7419,7 +7385,7 @@
         <v>13</v>
       </c>
       <c r="N2" s="78" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O2" s="77" t="s">
         <v>14</v>
@@ -7433,98 +7399,98 @@
     </row>
     <row r="3" spans="1:17" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>362</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>364</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H3" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>517</v>
-      </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="O3" s="14" t="s">
         <v>370</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>371</v>
       </c>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>489</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>490</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>491</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>523</v>
-      </c>
-      <c r="K4" s="14" t="s">
+      <c r="L4" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="M4" s="15" t="s">
         <v>493</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="M4" s="15" t="s">
+      <c r="N4" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>494</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>495</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>

</xml_diff>